<commit_message>
this model -> gap 11 X
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>400</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.825</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gap 10 X , gap 11 애매
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.825</v>
+        <v>0.925</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.175</v>
+        <v>0.075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gap 12도 애 매
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.925</v>
+        <v>0.95</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.075</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
this model gap 13 ->very good
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yes new model 1_0 -> CL (gap12) 100%
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,10 +445,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
5000_3 model in pipe_1 -> deadlock 조금
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yes new model1_0 success
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_3/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_3_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.95</v>
+        <v>0.975</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>